<commit_message>
Changed to IconButtons, new assets
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000B3EDE-BB5D-4EBF-9543-A9D09C5CE61C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AA05E0-285D-40FC-AE47-D5454EC51B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Flutter.dev introduction, playing with assets, buttons, containers, stacks | Found here: https://github.com/leono93/flutter-project</t>
+  </si>
+  <si>
+    <t>Routing, styling, invoking classes. Updates found at https://github.com/leono93/flutter-project</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +845,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -852,18 +855,22 @@
       <c r="B7" s="41">
         <v>10</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="41">
+        <v>15</v>
+      </c>
       <c r="D7" s="28">
         <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="G7" s="93" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Splash screen, icon update
Added splash screen, updated to higher res and bordered icons
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AA05E0-285D-40FC-AE47-D5454EC51B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46105995-298B-4EB4-817E-0C6EE102FC9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,7 +845,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,11 +856,11 @@
         <v>10</v>
       </c>
       <c r="C7" s="41">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="28">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>13</v>
@@ -870,7 +870,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hive basis, resource guide icons
Added basis for Hive integration, added shaded icons for class resource guides
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76953E2-42AC-414C-A824-7BBD8D0CC75F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F057ACD-4D91-4810-A020-B1BB05FE6DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -72,16 +72,19 @@
     <t>None // Worked on R&amp;D course</t>
   </si>
   <si>
-    <t>Creating + implementing splash screen, creating higher resolution icons + bordering them, looking into Firebase</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flutter.dev introduction, playing with assets, buttons, containers, stacks </t>
   </si>
   <si>
-    <t>Routing, styling, invoking classes</t>
-  </si>
-  <si>
     <t>https://github.com/leono93/flutter-project</t>
+  </si>
+  <si>
+    <t>Creating + implementing splash screen, creating higher resolution icons + bordering them, class titles with proper font</t>
+  </si>
+  <si>
+    <t>Routing, styling, creating and invoking existing classes based on each World of Warcraft class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking into noSQL options for this app and fending off error after error trying to implement them. Did not get much actual work done. </t>
   </si>
 </sst>
 </file>
@@ -743,7 +746,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +766,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="E1" s="95" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -854,14 +857,14 @@
         <v>8</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="91" t="s">
         <v>7</v>
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,14 +882,14 @@
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="93" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -897,27 +900,33 @@
         <v>10</v>
       </c>
       <c r="C8" s="41">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="28">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>44119</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
+      <c r="B9" s="41">
+        <v>10</v>
+      </c>
+      <c r="C9" s="41">
+        <v>16</v>
+      </c>
       <c r="D9" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12">

</xml_diff>

<commit_message>
Partially working nodeJS backend
Authentication = ok
GET = not yet ok
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F057ACD-4D91-4810-A020-B1BB05FE6DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C59E46-734C-4246-9FC6-DC9D1B32383E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -75,16 +75,19 @@
     <t xml:space="preserve">Flutter.dev introduction, playing with assets, buttons, containers, stacks </t>
   </si>
   <si>
-    <t>https://github.com/leono93/flutter-project</t>
-  </si>
-  <si>
     <t>Creating + implementing splash screen, creating higher resolution icons + bordering them, class titles with proper font</t>
   </si>
   <si>
     <t>Routing, styling, creating and invoking existing classes based on each World of Warcraft class</t>
   </si>
   <si>
-    <t xml:space="preserve">Looking into noSQL options for this app and fending off error after error trying to implement them. Did not get much actual work done. </t>
+    <t>Looking into noSQL options for this app and fending off error after error trying to implement them. Implemented basis of Hive</t>
+  </si>
+  <si>
+    <t>https://github.com/leono93/world-of-warcraft-pocket-buddy</t>
+  </si>
+  <si>
+    <t>Reading Blizzard API documentation and public resources on it as well as NodeJS implementation and libraries</t>
   </si>
 </sst>
 </file>
@@ -746,7 +749,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +769,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="E1" s="95" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -864,7 +867,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -882,14 +885,14 @@
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="93" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -907,7 +910,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,30 +928,40 @@
         <v>6</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>44120</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
+      <c r="B10" s="42">
+        <v>10</v>
+      </c>
+      <c r="C10" s="42">
+        <v>14</v>
+      </c>
       <c r="D10" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44123</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="43">
+        <v>11</v>
+      </c>
+      <c r="C11" s="43">
+        <v>16</v>
+      </c>
       <c r="D11" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fixed endpoints and parameters
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C59E46-734C-4246-9FC6-DC9D1B32383E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A67B623-BD1F-423E-A073-9D546E80A510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Reading Blizzard API documentation and public resources on it as well as NodeJS implementation and libraries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementing Blizzard.js library before making my own API endpoints. Requests to Blizzard API work after fixing outdated endpoints </t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +966,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">

</xml_diff>

<commit_message>
Fetch and display dummy data
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C64A0A-77F0-484F-BBEA-9953018B80E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DBD4D2-2859-48DB-B527-83655668E1B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -93,7 +93,13 @@
     <t xml:space="preserve">Implementing Blizzard.js library before making my own API endpoints. Requests to Blizzard API work after fixing outdated endpoints </t>
   </si>
   <si>
-    <t>Looking into the Flutter http package and testing example http calls and how to map the results</t>
+    <t>Fixed broken build and worked on R&amp;D course</t>
+  </si>
+  <si>
+    <t>Looking into the Flutter http package and testing example http calls to dummy JSON data</t>
+  </si>
+  <si>
+    <t>Figuring out how to map example JSON data. Also fixing endpoints for item + character retrieval from Blizzard API</t>
   </si>
 </sst>
 </file>
@@ -460,7 +466,7 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,7 +761,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +879,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -898,7 +904,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -988,44 +994,58 @@
         <v>4</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>44125</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="44">
+        <v>11</v>
+      </c>
+      <c r="C13" s="44">
+        <v>12</v>
+      </c>
       <c r="D13" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>44126</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="44">
+        <v>11</v>
+      </c>
+      <c r="C14" s="44">
+        <v>15</v>
+      </c>
       <c r="D14" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>44127</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="45">
+        <v>10</v>
+      </c>
+      <c r="C15" s="45">
+        <v>16</v>
+      </c>
       <c r="D15" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" s="7"/>
     </row>

</xml_diff>

<commit_message>
ListViews for each class list
Added ListViews for each class list, and add character button. Also fixed some redirects.
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE4A93E-0B8A-4CF0-8C6C-61830EA23F71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66DEC1E-3711-4C18-8F27-447A29045586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Fetching and mapping example JSON data. Also fixing endpoints for item + character retrieval from Blizzard API</t>
+  </si>
+  <si>
+    <t>Testing new token fetching and updating, planning out what and how to display from character info on frontend</t>
+  </si>
+  <si>
+    <t>Adding resource redirects to each respective class, styling for ListViews when character list is implemented</t>
   </si>
 </sst>
 </file>
@@ -761,7 +767,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +885,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -904,7 +910,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1041,25 +1047,33 @@
         <v>10</v>
       </c>
       <c r="C15" s="45">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D15" s="32">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E15" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="51">
         <v>44130</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
+      <c r="B16" s="52">
+        <v>9</v>
+      </c>
+      <c r="C16" s="52">
+        <v>15</v>
+      </c>
       <c r="D16" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="54"/>
+        <v>6</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="55">

</xml_diff>

<commit_message>
Info page to each class
Info pages and descriptions added
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66DEC1E-3711-4C18-8F27-447A29045586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B233F9-126B-43FA-9D06-E0B516C5CFA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Adding resource redirects to each respective class, styling for ListViews when character list is implemented</t>
+  </si>
+  <si>
+    <t>Added info button + pages to each class with respective descriptions</t>
   </si>
 </sst>
 </file>
@@ -767,7 +770,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +888,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -910,7 +913,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1079,13 +1082,19 @@
       <c r="A17" s="55">
         <v>44131</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="B17" s="46">
+        <v>10</v>
+      </c>
+      <c r="C17" s="46">
+        <v>15</v>
+      </c>
       <c r="D17" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="56"/>
+        <v>5</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="55">

</xml_diff>

<commit_message>
Moved external resources to class descriptions
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B233F9-126B-43FA-9D06-E0B516C5CFA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988129F6-866E-42A5-9339-C9A213FFE755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
     <t>Adding resource redirects to each respective class, styling for ListViews when character list is implemented</t>
   </si>
   <si>
-    <t>Added info button + pages to each class with respective descriptions</t>
+    <t xml:space="preserve">Added info button + pages to each class with respective descriptions. Changed text styling, added assets for each spec. </t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Character model, form, ListView
Added Hive -> Character model, add character form, display ListView in Warrior class
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988129F6-866E-42A5-9339-C9A213FFE755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D86F4-F6FF-4564-AB37-F1F8517B46B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -770,7 +770,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1100,11 +1100,15 @@
       <c r="A18" s="55">
         <v>44132</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
+      <c r="B18" s="46">
+        <v>9</v>
+      </c>
+      <c r="C18" s="46">
+        <v>15</v>
+      </c>
       <c r="D18" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E18" s="56"/>
     </row>

</xml_diff>

<commit_message>
Added unstyled bottom navbar
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D86F4-F6FF-4564-AB37-F1F8517B46B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB4B9A-374D-4862-9CFA-A1348E0FFD1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t xml:space="preserve">Added info button + pages to each class with respective descriptions. Changed text styling, added assets for each spec. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looked into SQLFlite options, minor style changes. </t>
+  </si>
+  <si>
+    <t>Spent a few hours playing with Hive but decided not to use it and reverted the changes (lack of documentation, many deprecations)</t>
+  </si>
+  <si>
+    <t>Planning out Raider.io API integration</t>
+  </si>
+  <si>
+    <t>Planned out content management more // had job interview on this day</t>
   </si>
 </sst>
 </file>
@@ -379,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -476,6 +488,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +783,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,6 +793,7 @@
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="120.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -859,6 +873,10 @@
       <c r="E5" s="19" t="s">
         <v>11</v>
       </c>
+      <c r="F5" s="96">
+        <f>SUM(D3:D5)</f>
+        <v>2</v>
+      </c>
       <c r="G5" s="89" t="s">
         <v>8</v>
       </c>
@@ -888,7 +906,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -913,7 +931,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -969,6 +987,10 @@
       <c r="E10" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="F10" s="96">
+        <f>SUM(D6:D10)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1059,6 +1081,10 @@
       <c r="E15" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="F15" s="96">
+        <f>SUM(D11:D15)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="51">
@@ -1078,7 +1104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="55">
         <v>44131</v>
       </c>
@@ -1096,7 +1122,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="55">
         <v>44132</v>
       </c>
@@ -1104,51 +1130,75 @@
         <v>9</v>
       </c>
       <c r="C18" s="46">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D18" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E18" s="56"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="55">
         <v>44133</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="B19" s="46">
+        <v>11</v>
+      </c>
+      <c r="C19" s="46">
+        <v>13</v>
+      </c>
       <c r="D19" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="56"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="57">
         <v>44134</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
+      <c r="B20" s="58">
+        <v>8</v>
+      </c>
+      <c r="C20" s="58">
+        <v>11</v>
+      </c>
       <c r="D20" s="59">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="60"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="96">
+        <f>SUM(D16:D20)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="61">
         <v>44137</v>
       </c>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
+      <c r="B21" s="62">
+        <v>9</v>
+      </c>
+      <c r="C21" s="62">
+        <v>13</v>
+      </c>
       <c r="D21" s="63">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="64"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="65">
         <v>44138</v>
       </c>
@@ -1160,7 +1210,7 @@
       </c>
       <c r="E22" s="66"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="65">
         <v>44139</v>
       </c>
@@ -1172,7 +1222,7 @@
       </c>
       <c r="E23" s="66"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="65">
         <v>44140</v>
       </c>
@@ -1184,7 +1234,7 @@
       </c>
       <c r="E24" s="66"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
         <v>44141</v>
       </c>
@@ -1195,8 +1245,12 @@
         <v>0</v>
       </c>
       <c r="E25" s="70"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="96">
+        <f>SUM(D21:D25)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="71">
         <v>44144</v>
       </c>
@@ -1208,7 +1262,7 @@
       </c>
       <c r="E26" s="74"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="75">
         <v>44145</v>
       </c>
@@ -1220,7 +1274,7 @@
       </c>
       <c r="E27" s="76"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="75">
         <v>44146</v>
       </c>
@@ -1232,7 +1286,7 @@
       </c>
       <c r="E28" s="76"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="75">
         <v>44147</v>
       </c>
@@ -1244,7 +1298,7 @@
       </c>
       <c r="E29" s="76"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="77">
         <v>44148</v>
       </c>
@@ -1255,8 +1309,12 @@
         <v>0</v>
       </c>
       <c r="E30" s="80"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="96">
+        <f>SUM(D26:D30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="81">
         <v>44151</v>
       </c>
@@ -1268,7 +1326,7 @@
       </c>
       <c r="E31" s="84"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="85">
         <v>44152</v>
       </c>
@@ -1280,7 +1338,7 @@
       </c>
       <c r="E32" s="86"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="85">
         <v>44153</v>
       </c>
@@ -1292,7 +1350,7 @@
       </c>
       <c r="E33" s="86"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="85">
         <v>44154</v>
       </c>
@@ -1304,7 +1362,7 @@
       </c>
       <c r="E34" s="86"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="87">
         <v>44155</v>
       </c>
@@ -1315,6 +1373,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="88"/>
+      <c r="F35" s="96">
+        <f>SUM(D31:D35)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Full realmlist + mapping
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB4B9A-374D-4862-9CFA-A1348E0FFD1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7179B-6801-41C1-821C-74D2486FA700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -117,10 +117,19 @@
     <t>Spent a few hours playing with Hive but decided not to use it and reverted the changes (lack of documentation, many deprecations)</t>
   </si>
   <si>
-    <t>Planning out Raider.io API integration</t>
-  </si>
-  <si>
     <t>Planned out content management more // had job interview on this day</t>
+  </si>
+  <si>
+    <t>Planning out Raider.io API integration, filtering relevant character information, creating bottom appbar for better navigation options</t>
+  </si>
+  <si>
+    <t>Worked on R&amp;D course</t>
+  </si>
+  <si>
+    <t>Worked on R&amp;D course // Finished now</t>
+  </si>
+  <si>
+    <t>Created EU realm list, search page</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,7 +503,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +798,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +921,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -931,7 +946,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1173,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="96">
         <f>SUM(D16:D20)</f>
@@ -1188,14 +1203,14 @@
         <v>9</v>
       </c>
       <c r="C21" s="62">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D21" s="63">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1208,7 +1223,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="66"/>
+      <c r="E22" s="66" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="65">
@@ -1220,19 +1237,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="66"/>
+      <c r="E23" s="66" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="65">
         <v>44140</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
+      <c r="B24" s="47">
+        <v>12</v>
+      </c>
+      <c r="C24" s="47">
+        <v>15</v>
+      </c>
       <c r="D24" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="66"/>
+        <v>3</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
@@ -1247,18 +1272,22 @@
       <c r="E25" s="70"/>
       <c r="F25" s="96">
         <f>SUM(D21:D25)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="71">
         <v>44144</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
+      <c r="B26" s="72">
+        <v>10</v>
+      </c>
+      <c r="C26" s="72">
+        <v>15</v>
+      </c>
       <c r="D26" s="73">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E26" s="74"/>
     </row>
@@ -1311,7 +1340,7 @@
       <c r="E30" s="80"/>
       <c r="F30" s="96">
         <f>SUM(D26:D30)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Retrieve, parse and map Raider IO API data
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7179B-6801-41C1-821C-74D2486FA700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A3096-0C18-473D-B4D0-01256BA919A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Created EU realm list, search page</t>
+  </si>
+  <si>
+    <t>Bottom NavBar styling, building realmlist to ListView with unique elements from array</t>
+  </si>
+  <si>
+    <t>Input fields for character and realm, realm selection, fetching the values of the input fields, some modifications for RaiderIO API</t>
   </si>
 </sst>
 </file>
@@ -797,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +927,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -946,7 +952,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1263,16 +1269,22 @@
       <c r="A25" s="67">
         <v>44141</v>
       </c>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
+      <c r="B25" s="68">
+        <v>10</v>
+      </c>
+      <c r="C25" s="68">
+        <v>14</v>
+      </c>
       <c r="D25" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="70"/>
+        <v>4</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="96">
         <f>SUM(D21:D25)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,16 +1292,18 @@
         <v>44144</v>
       </c>
       <c r="B26" s="72">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" s="72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" s="73">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E26" s="74"/>
+        <v>7</v>
+      </c>
+      <c r="E26" s="74" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="75">
@@ -1340,7 +1354,7 @@
       <c r="E30" s="80"/>
       <c r="F30" s="96">
         <f>SUM(D26:D30)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
URL parameters based on input
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BB35D2-A754-4C71-80E2-0F9FEB49D9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DD2776-EAF2-430B-8DDD-F77191356607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -129,13 +129,19 @@
     <t>Worked on R&amp;D course // Finished now</t>
   </si>
   <si>
-    <t>Created EU realm list, search page</t>
-  </si>
-  <si>
     <t>Bottom NavBar styling, building realmlist to ListView with unique elements from array</t>
   </si>
   <si>
     <t>Input fields for character and realm, realm selection, fetching the values of the input fields, some modifications for RaiderIO API</t>
+  </si>
+  <si>
+    <t>Dynamic API requests and connecting input fields to character fetch. Dealing with problems of passing data from stless/stful widget</t>
+  </si>
+  <si>
+    <t>Hours:</t>
+  </si>
+  <si>
+    <t>Created EU realm list, search page &amp; form</t>
   </si>
 </sst>
 </file>
@@ -803,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,6 +886,9 @@
       <c r="E4" s="17" t="s">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -990,6 +999,9 @@
       <c r="E9" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -1084,6 +1096,9 @@
       <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -1178,6 +1193,9 @@
       <c r="E19" s="56" t="s">
         <v>25</v>
       </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="57">
@@ -1262,7 +1280,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="66" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="96">
         <f>SUM(D21:D25)</f>
@@ -1302,7 +1323,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="74" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1319,7 +1340,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E27" s="76"/>
+      <c r="E27" s="76" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="75">
@@ -1344,6 +1367,9 @@
         <v>0</v>
       </c>
       <c r="E29" s="76"/>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="77">
@@ -1408,6 +1434,9 @@
         <v>0</v>
       </c>
       <c r="E34" s="86"/>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="87">

</xml_diff>

<commit_message>
Realm ListView to GridView
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DD2776-EAF2-430B-8DDD-F77191356607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF9A859-46BC-4A34-84C6-9C6891CA03C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Created EU realm list, search page &amp; form</t>
+  </si>
+  <si>
+    <t>Trying to fix some issues with displaying the parsed JSON data</t>
+  </si>
+  <si>
+    <t>Maalisuora Event</t>
   </si>
 </sst>
 </file>
@@ -810,7 +816,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +942,7 @@
       </c>
       <c r="H6" s="92">
         <f>SUM(D3:D68)</f>
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,7 +967,7 @@
       </c>
       <c r="H7" s="94">
         <f>H5-H6</f>
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1348,13 +1354,19 @@
       <c r="A28" s="75">
         <v>44146</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
+      <c r="B28" s="48">
+        <v>10</v>
+      </c>
+      <c r="C28" s="48">
+        <v>13</v>
+      </c>
       <c r="D28" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="76"/>
+        <v>3</v>
+      </c>
+      <c r="E28" s="76" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="75">
@@ -1366,7 +1378,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="76"/>
+      <c r="E29" s="76" t="s">
+        <v>37</v>
+      </c>
       <c r="F29" t="s">
         <v>34</v>
       </c>
@@ -1384,7 +1398,7 @@
       <c r="E30" s="80"/>
       <c r="F30" s="96">
         <f>SUM(D26:D30)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Style changes, sqflite initialized
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5064E5A-D453-4576-B721-EF8FFB836E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30496FB1-10A6-4A1B-9F44-43587310E3C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Style changes across the board; realm selection changes + styling</t>
+  </si>
+  <si>
+    <t>Honestly, wasted a few hours on (almost) meaningless styling. At least it looks okay.</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6C292"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -462,7 +471,6 @@
     <xf numFmtId="1" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -475,7 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -512,8 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -522,6 +527,15 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,6 +544,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC6C292"/>
       <color rgb="FF8695DE"/>
       <color rgb="FFA5D9E3"/>
       <color rgb="FFD788F0"/>
@@ -813,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +851,7 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="91" t="s">
         <v>15</v>
       </c>
     </row>
@@ -879,14 +894,14 @@
       <c r="A4" s="16">
         <v>44112</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="37">
         <v>12</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="37">
         <v>13</v>
       </c>
       <c r="D4" s="25">
-        <f t="shared" ref="D4:D35" si="0">C4-B4</f>
+        <f t="shared" ref="D4:D40" si="0">C4-B4</f>
         <v>1</v>
       </c>
       <c r="E4" s="17" t="s">
@@ -900,8 +915,8 @@
       <c r="A5" s="18">
         <v>44113</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -909,14 +924,14 @@
       <c r="E5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="96">
+      <c r="F5" s="92">
         <f>SUM(D3:D5)</f>
         <v>2</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="90">
+      <c r="H5" s="86">
         <v>200</v>
       </c>
     </row>
@@ -924,10 +939,10 @@
       <c r="A6" s="8">
         <v>44116</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="39">
         <v>8</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>16</v>
       </c>
       <c r="D6" s="27">
@@ -937,22 +952,22 @@
       <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="G6" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="92">
+      <c r="H6" s="88">
         <f>SUM(D3:D68)</f>
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>44117</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="40">
         <v>10</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>16</v>
       </c>
       <c r="D7" s="28">
@@ -962,22 +977,22 @@
       <c r="E7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="93" t="s">
+      <c r="G7" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="94">
+      <c r="H7" s="90">
         <f>H5-H6</f>
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>44118</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="40">
         <v>10</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>16</v>
       </c>
       <c r="D8" s="28">
@@ -992,10 +1007,10 @@
       <c r="A9" s="10">
         <v>44119</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="40">
         <v>10</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="40">
         <v>16</v>
       </c>
       <c r="D9" s="28">
@@ -1013,10 +1028,10 @@
       <c r="A10" s="12">
         <v>44120</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="41">
         <v>10</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="41">
         <v>14</v>
       </c>
       <c r="D10" s="29">
@@ -1026,7 +1041,7 @@
       <c r="E10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="96">
+      <c r="F10" s="92">
         <f>SUM(D6:D10)</f>
         <v>30</v>
       </c>
@@ -1035,10 +1050,10 @@
       <c r="A11" s="2">
         <v>44123</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="42">
         <v>11</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="42">
         <v>16</v>
       </c>
       <c r="D11" s="30">
@@ -1053,10 +1068,10 @@
       <c r="A12" s="4">
         <v>44124</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="43">
         <v>11</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="43">
         <v>15</v>
       </c>
       <c r="D12" s="31">
@@ -1071,10 +1086,10 @@
       <c r="A13" s="4">
         <v>44125</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="43">
         <v>11</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="43">
         <v>12</v>
       </c>
       <c r="D13" s="31">
@@ -1089,10 +1104,10 @@
       <c r="A14" s="4">
         <v>44126</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="43">
         <v>11</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="43">
         <v>15</v>
       </c>
       <c r="D14" s="31">
@@ -1110,10 +1125,10 @@
       <c r="A15" s="6">
         <v>44127</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B15" s="44">
         <v>10</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="44">
         <v>13</v>
       </c>
       <c r="D15" s="32">
@@ -1123,80 +1138,80 @@
       <c r="E15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="96">
+      <c r="F15" s="92">
         <f>SUM(D11:D15)</f>
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="51">
+      <c r="A16" s="49">
         <v>44130</v>
       </c>
-      <c r="B16" s="52">
+      <c r="B16" s="50">
         <v>9</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="50">
         <v>15</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="51">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="52" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="55">
+      <c r="A17" s="53">
         <v>44131</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B17" s="45">
         <v>10</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="45">
         <v>15</v>
       </c>
       <c r="D17" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="54" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="55">
+      <c r="A18" s="53">
         <v>44132</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18" s="45">
         <v>9</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <v>13</v>
       </c>
       <c r="D18" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="55">
+      <c r="A19" s="53">
         <v>44133</v>
       </c>
-      <c r="B19" s="46">
+      <c r="B19" s="45">
         <v>11</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <v>13</v>
       </c>
       <c r="D19" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="54" t="s">
         <v>24</v>
       </c>
       <c r="F19" t="s">
@@ -1204,88 +1219,88 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="57">
+      <c r="A20" s="55">
         <v>44134</v>
       </c>
-      <c r="B20" s="58">
+      <c r="B20" s="56">
         <v>8</v>
       </c>
-      <c r="C20" s="58">
+      <c r="C20" s="56">
         <v>11</v>
       </c>
-      <c r="D20" s="59">
+      <c r="D20" s="57">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="96">
+      <c r="F20" s="92">
         <f>SUM(D16:D20)</f>
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="61">
+      <c r="A21" s="59">
         <v>44137</v>
       </c>
-      <c r="B21" s="62">
+      <c r="B21" s="60">
         <v>9</v>
       </c>
-      <c r="C21" s="62">
+      <c r="C21" s="60">
         <v>15</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="61">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E21" s="64" t="s">
+      <c r="E21" s="62" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="65">
+      <c r="A22" s="63">
         <v>44138</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="66" t="s">
+      <c r="E22" s="64" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="65">
+      <c r="A23" s="63">
         <v>44139</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="E23" s="64" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="65">
+      <c r="A24" s="63">
         <v>44140</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B24" s="46">
         <v>12</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="46">
         <v>15</v>
       </c>
       <c r="D24" s="34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="64" t="s">
         <v>34</v>
       </c>
       <c r="F24" t="s">
@@ -1293,92 +1308,92 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="67">
+      <c r="A25" s="65">
         <v>44141</v>
       </c>
-      <c r="B25" s="68">
+      <c r="B25" s="66">
         <v>10</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="66">
         <v>14</v>
       </c>
-      <c r="D25" s="69">
+      <c r="D25" s="67">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="96">
+      <c r="F25" s="92">
         <f>SUM(D21:D25)</f>
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="71">
+      <c r="A26" s="69">
         <v>44144</v>
       </c>
-      <c r="B26" s="72">
+      <c r="B26" s="70">
         <v>9</v>
       </c>
-      <c r="C26" s="72">
+      <c r="C26" s="70">
         <v>16</v>
       </c>
-      <c r="D26" s="73">
+      <c r="D26" s="71">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="72" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="75">
+      <c r="A27" s="73">
         <v>44145</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="47">
         <v>10</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="47">
         <v>16</v>
       </c>
       <c r="D27" s="35">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E27" s="76" t="s">
+      <c r="E27" s="74" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="75">
+      <c r="A28" s="73">
         <v>44146</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="47">
         <v>10</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="47">
         <v>13</v>
       </c>
       <c r="D28" s="35">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E28" s="76" t="s">
+      <c r="E28" s="74" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="75">
+      <c r="A29" s="73">
         <v>44147</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="76" t="s">
+      <c r="E29" s="74" t="s">
         <v>36</v>
       </c>
       <c r="F29" t="s">
@@ -1386,91 +1401,164 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="77">
+      <c r="A30" s="75">
         <v>44148</v>
       </c>
-      <c r="B30" s="78">
+      <c r="B30" s="76">
         <v>12</v>
       </c>
-      <c r="C30" s="78">
+      <c r="C30" s="76">
         <v>14</v>
       </c>
-      <c r="D30" s="79">
+      <c r="D30" s="77">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E30" s="80" t="s">
+      <c r="E30" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="96">
+      <c r="F30" s="92">
         <f>SUM(D26:D30)</f>
         <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="81">
+      <c r="A31" s="79">
         <v>44151</v>
       </c>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="83">
+      <c r="B31" s="80">
+        <v>12</v>
+      </c>
+      <c r="C31" s="80">
+        <v>15</v>
+      </c>
+      <c r="D31" s="81">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" s="82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="83">
+        <v>44152</v>
+      </c>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="84"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="85">
-        <v>44152</v>
-      </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="36">
+      <c r="E32" s="84"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="83">
+        <v>44153</v>
+      </c>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="86"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="85">
-        <v>44153</v>
-      </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="36">
+      <c r="E33" s="84"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="83">
+        <v>44154</v>
+      </c>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="86"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="85">
-        <v>44154</v>
-      </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="86"/>
+      <c r="E34" s="84"/>
       <c r="F34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="87">
+      <c r="A35" s="83">
         <v>44155</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="37">
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="88"/>
-      <c r="F35" s="96">
+      <c r="E35" s="84"/>
+      <c r="F35" s="92">
         <f>SUM(D31:D35)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="93">
+        <v>44158</v>
+      </c>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="95">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="94"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="96">
+        <v>44159</v>
+      </c>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="98">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="97"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="96">
+        <v>44160</v>
+      </c>
+      <c r="B38" s="97"/>
+      <c r="C38" s="97"/>
+      <c r="D38" s="98">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="97"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="96">
+        <v>44161</v>
+      </c>
+      <c r="B39" s="97"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="98">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="97"/>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="99">
+        <v>44162</v>
+      </c>
+      <c r="B40" s="100"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="101">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="100"/>
+      <c r="F40" s="92">
+        <f>SUM(D36:D40)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Database expanded,  form style changes
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC644E-0BA0-4A03-8BEE-07497656607E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9448358-F12D-4185-843F-98A409A79400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -153,7 +153,10 @@
     <t>Honestly, wasted a few hours on (almost) meaningless styling. At least it looks okay.</t>
   </si>
   <si>
-    <t>Creating SQFLite implementation for character storage + CRUD functions</t>
+    <t>Creating SQFLite implementation for character storage + CRUD methods + routing from existing pages</t>
+  </si>
+  <si>
+    <t>Database modifications, adding fields and modifying form</t>
   </si>
 </sst>
 </file>
@@ -833,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +963,7 @@
       </c>
       <c r="H6" s="88">
         <f>SUM(D3:D68)</f>
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -985,7 +988,7 @@
       </c>
       <c r="H7" s="90">
         <f>H5-H6</f>
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,14 +1451,14 @@
         <v>44152</v>
       </c>
       <c r="B32" s="48">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="48">
         <v>16</v>
       </c>
       <c r="D32" s="36">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32" s="84" t="s">
         <v>39</v>
@@ -1465,13 +1468,19 @@
       <c r="A33" s="83">
         <v>44153</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
+      <c r="B33" s="48">
+        <v>12</v>
+      </c>
+      <c r="C33" s="48">
+        <v>16</v>
+      </c>
       <c r="D33" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="84"/>
+        <v>4</v>
+      </c>
+      <c r="E33" s="84" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="83">
@@ -1501,7 +1510,7 @@
       <c r="E35" s="84"/>
       <c r="F35" s="92">
         <f>SUM(D31:D35)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final commit for project review
</commit_message>
<xml_diff>
--- a/project-docs/Project WTT.xlsx
+++ b/project-docs/Project WTT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Flutter\newApp\flutter-practice\project-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F44010-1696-48AE-BF81-DA70CE49342E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562EA0CA-208F-4CFF-A377-B3F6E7AF0737}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Worktime MOBILE APP PROJECT</t>
   </si>
@@ -168,7 +168,40 @@
     <t xml:space="preserve">Mostly spent time cleaning up the code. A lot of early code was a mess in terms of widgets/widget wrapping </t>
   </si>
   <si>
-    <t>Rewrote each unique class  widgets</t>
+    <t>Rewrote each unique class widgets, fixed some errors with fetching assets that broke the build</t>
+  </si>
+  <si>
+    <t>Had to fix some mistakes for the R&amp;D course work</t>
+  </si>
+  <si>
+    <t>Changes to CharacterList cards, tried some dropdownfield library. Characters now display info according to faction</t>
+  </si>
+  <si>
+    <t>Replanning what to do with the class widgets to make the information more relevant. Will display spec info and covenant info also</t>
+  </si>
+  <si>
+    <t>Rewriting the API call/JSON part of the code as what I currently had did not work out as I want it to - not finished yet</t>
+  </si>
+  <si>
+    <t>Finished rewriting Raider.IO API call / mapped response to ListView</t>
+  </si>
+  <si>
+    <t>Rewrote a big chunk of the class widgets. No longer showing classes from character list as it seems unnecessary, rather more info</t>
+  </si>
+  <si>
+    <t>Changed database and remolled the code accordingly. More details about characters now.</t>
+  </si>
+  <si>
+    <t>Restyling character search page, testing with a few test widgets</t>
+  </si>
+  <si>
+    <t>Rearranging the main widgets since some parts remain unfinished until after the project is done</t>
+  </si>
+  <si>
+    <t>Lots of changes, changing up links to match new Shadowlands data, looking more into Blizzard API after updates</t>
+  </si>
+  <si>
+    <t>Finalizing project for review; styling changes, different navigation (filtered out the classes) and consistency updates</t>
   </si>
 </sst>
 </file>
@@ -201,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +331,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5F9782"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -451,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -554,6 +599,38 @@
     <xf numFmtId="14" fontId="0" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="16" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="18" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,6 +639,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF5F9782"/>
+      <color rgb="FF93EFEB"/>
+      <color rgb="FFF88A8A"/>
       <color rgb="FFC6C292"/>
       <color rgb="FF8695DE"/>
       <color rgb="FFA5D9E3"/>
@@ -569,7 +649,6 @@
       <color rgb="FFBADE8E"/>
       <color rgb="FFE27870"/>
       <color rgb="FFE24A4A"/>
-      <color rgb="FFEFABAB"/>
     </mruColors>
   </colors>
   <extLst>
@@ -846,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,7 +1054,7 @@
       </c>
       <c r="H6" s="88">
         <f>SUM(D3:D68)</f>
-        <v>127</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,7 +1079,7 @@
       </c>
       <c r="H7" s="90">
         <f>H5-H6</f>
-        <v>73</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1108,11 +1187,11 @@
         <v>11</v>
       </c>
       <c r="C13" s="43">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
@@ -1123,14 +1202,14 @@
         <v>44126</v>
       </c>
       <c r="B14" s="43">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="43">
         <v>15</v>
       </c>
       <c r="D14" s="31">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>20</v>
@@ -1158,7 +1237,7 @@
       </c>
       <c r="F15" s="92">
         <f>SUM(D11:D15)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1205,11 +1284,11 @@
         <v>9</v>
       </c>
       <c r="C18" s="45">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18" s="33">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" s="54" t="s">
         <v>25</v>
@@ -1255,7 +1334,7 @@
       </c>
       <c r="F20" s="92">
         <f>SUM(D16:D20)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1312,11 +1391,11 @@
         <v>12</v>
       </c>
       <c r="C24" s="46">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" s="34">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" s="64" t="s">
         <v>34</v>
@@ -1344,7 +1423,7 @@
       </c>
       <c r="F25" s="92">
         <f>SUM(D21:D25)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,14 +1449,14 @@
         <v>44145</v>
       </c>
       <c r="B27" s="47">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="47">
         <v>16</v>
       </c>
       <c r="D27" s="35">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E27" s="74" t="s">
         <v>32</v>
@@ -1391,11 +1470,11 @@
         <v>10</v>
       </c>
       <c r="C28" s="47">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D28" s="35">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28" s="74" t="s">
         <v>35</v>
@@ -1437,7 +1516,7 @@
       </c>
       <c r="F30" s="92">
         <f>SUM(D26:D30)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1448,11 +1527,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="80">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="81">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="82" t="s">
         <v>38</v>
@@ -1466,11 +1545,11 @@
         <v>10</v>
       </c>
       <c r="C32" s="48">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="36">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E32" s="84" t="s">
         <v>39</v>
@@ -1484,11 +1563,11 @@
         <v>12</v>
       </c>
       <c r="C33" s="48">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D33" s="36">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E33" s="84" t="s">
         <v>40</v>
@@ -1523,18 +1602,18 @@
         <v>13</v>
       </c>
       <c r="C35" s="48">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D35" s="36">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E35" s="84" t="s">
         <v>42</v>
       </c>
       <c r="F35" s="92">
         <f>SUM(D31:D35)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1563,11 +1642,11 @@
         <v>10</v>
       </c>
       <c r="C37" s="97">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D37" s="98">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E37" s="97" t="s">
         <v>44</v>
@@ -1583,7 +1662,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="97"/>
+      <c r="E38" s="97" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="96">
@@ -1604,16 +1685,277 @@
       <c r="A40" s="99">
         <v>44162</v>
       </c>
-      <c r="B40" s="100"/>
-      <c r="C40" s="100"/>
+      <c r="B40" s="100">
+        <v>11</v>
+      </c>
+      <c r="C40" s="100">
+        <v>14</v>
+      </c>
       <c r="D40" s="101">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="100"/>
+        <v>3</v>
+      </c>
+      <c r="E40" s="100" t="s">
+        <v>46</v>
+      </c>
       <c r="F40" s="92">
         <f>SUM(D36:D40)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="102">
+        <v>44165</v>
+      </c>
+      <c r="B41" s="103">
+        <v>9</v>
+      </c>
+      <c r="C41" s="103">
+        <v>12</v>
+      </c>
+      <c r="D41" s="104">
+        <f t="shared" ref="D41:D45" si="1">C41-B41</f>
+        <v>3</v>
+      </c>
+      <c r="E41" s="103" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="105">
+        <v>44166</v>
+      </c>
+      <c r="B42" s="106">
+        <v>9</v>
+      </c>
+      <c r="C42" s="106">
+        <v>14</v>
+      </c>
+      <c r="D42" s="107">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E42" s="106" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="105">
+        <v>44167</v>
+      </c>
+      <c r="B43" s="106">
+        <v>9</v>
+      </c>
+      <c r="C43" s="106">
+        <v>15</v>
+      </c>
+      <c r="D43" s="107">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E43" s="106" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="105">
+        <v>44168</v>
+      </c>
+      <c r="B44" s="106"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="107">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="106"/>
+      <c r="F44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="105">
+        <v>44169</v>
+      </c>
+      <c r="B45" s="108"/>
+      <c r="C45" s="108"/>
+      <c r="D45" s="109">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="108"/>
+      <c r="F45" s="92">
+        <f>SUM(D41:D45)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="119">
+        <v>44172</v>
+      </c>
+      <c r="B46" s="116">
         <v>8</v>
+      </c>
+      <c r="C46" s="110">
+        <v>15</v>
+      </c>
+      <c r="D46" s="111">
+        <f t="shared" ref="D46:D50" si="2">C46-B46</f>
+        <v>7</v>
+      </c>
+      <c r="E46" s="110" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="120">
+        <v>44173</v>
+      </c>
+      <c r="B47" s="117">
+        <v>9</v>
+      </c>
+      <c r="C47" s="112">
+        <v>15</v>
+      </c>
+      <c r="D47" s="113">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E47" s="112" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="120">
+        <v>44174</v>
+      </c>
+      <c r="B48" s="117">
+        <v>9</v>
+      </c>
+      <c r="C48" s="112">
+        <v>14</v>
+      </c>
+      <c r="D48" s="113">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E48" s="112" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="120">
+        <v>44175</v>
+      </c>
+      <c r="B49" s="117">
+        <v>9</v>
+      </c>
+      <c r="C49" s="112">
+        <v>16</v>
+      </c>
+      <c r="D49" s="113">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E49" s="112" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="121">
+        <v>44176</v>
+      </c>
+      <c r="B50" s="118"/>
+      <c r="C50" s="114"/>
+      <c r="D50" s="115">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="114"/>
+      <c r="F50" s="92">
+        <f>SUM(D46:D50)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="122">
+        <v>44179</v>
+      </c>
+      <c r="B51" s="123">
+        <v>8</v>
+      </c>
+      <c r="C51" s="124">
+        <v>16</v>
+      </c>
+      <c r="D51" s="125">
+        <f t="shared" ref="D51:D55" si="3">C51-B51</f>
+        <v>8</v>
+      </c>
+      <c r="E51" s="124" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="126">
+        <v>44180</v>
+      </c>
+      <c r="B52" s="127"/>
+      <c r="C52" s="128"/>
+      <c r="D52" s="129">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="128"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="126">
+        <v>44181</v>
+      </c>
+      <c r="B53" s="127">
+        <v>8</v>
+      </c>
+      <c r="C53" s="128">
+        <v>16</v>
+      </c>
+      <c r="D53" s="129">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="E53" s="128" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="126">
+        <v>44182</v>
+      </c>
+      <c r="B54" s="127"/>
+      <c r="C54" s="128"/>
+      <c r="D54" s="129">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="128"/>
+      <c r="F54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="130">
+        <v>44183</v>
+      </c>
+      <c r="B55" s="131"/>
+      <c r="C55" s="132"/>
+      <c r="D55" s="133">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="132"/>
+      <c r="F55" s="92">
+        <f>SUM(D51:D55)</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>